<commit_message>
visualizations built, BERT confirmed working
</commit_message>
<xml_diff>
--- a/data_corpus/Fully Duplicate ReorderedColumns 3.xlsx
+++ b/data_corpus/Fully Duplicate ReorderedColumns 3.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE0C25C-231D-484A-A810-801F98382AFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="25600" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,6 +88,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,13 +118,16 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -171,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,9 +209,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,6 +261,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -414,16 +453,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -443,7 +482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2363</v>
       </c>
@@ -463,181 +502,181 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
+        <v>6948</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1252</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>8436</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1404</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>8796</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1690</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>9197</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1690</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>9338</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1690</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6399</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1243</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>3135</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
         <v>498</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="F9" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>4899</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
         <v>658</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="F10" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>5691</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
         <v>1132</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F5" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>6399</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1243</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6948</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1252</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>8436</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1404</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8796</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1690</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9197</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1690</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9338</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1690</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F11" s="1">
         <v>50</v>
@@ -649,16 +688,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,7 +717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -698,7 +737,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -718,7 +757,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -738,7 +777,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -758,7 +797,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -778,7 +817,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -798,7 +837,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -818,7 +857,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -838,7 +877,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -858,7 +897,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -884,12 +923,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>